<commit_message>
Fixed a bug in Calvin2011.txt. Extra space "Calvin 2011", not "Calvin2011".
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/Calvin2011/SouthAfricaDataWorkbook.xlsx
+++ b/data/Excel Workbooks/Calvin2011/SouthAfricaDataWorkbook.xlsx
@@ -978,7 +978,7 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Calvin 2011</t>
+    <t>Calvin2011</t>
   </si>
 </sst>
 </file>
@@ -4190,11 +4190,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112830024"/>
-        <c:axId val="-2105977480"/>
+        <c:axId val="-2102626344"/>
+        <c:axId val="-2102669976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2112830024"/>
+        <c:axId val="-2102626344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4216,19 +4216,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105977480"/>
+        <c:crossAx val="-2102669976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2105977480"/>
+        <c:axId val="-2102669976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4250,14 +4249,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112830024"/>
+        <c:crossAx val="-2102626344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5138,23 +5136,23 @@
         <v>4490451.7342776405</v>
       </c>
       <c r="G12" s="71">
-        <f>A12-$A$12</f>
+        <f t="shared" ref="G12:G32" si="0">A12-$A$12</f>
         <v>0</v>
       </c>
       <c r="H12" s="21">
-        <f>B12/$B$12</f>
+        <f t="shared" ref="H12:H32" si="1">B12/$B$12</f>
         <v>1</v>
       </c>
       <c r="I12" s="5">
-        <f>C12/$C$12</f>
+        <f t="shared" ref="I12:I32" si="2">C12/$C$12</f>
         <v>1</v>
       </c>
       <c r="J12" s="5">
-        <f>D12/$D$12</f>
+        <f t="shared" ref="J12:J32" si="3">D12/$D$12</f>
         <v>1</v>
       </c>
       <c r="K12" s="5">
-        <f t="shared" ref="K12:K32" si="0">E12/$E$12</f>
+        <f t="shared" ref="K12:K32" si="4">E12/$E$12</f>
         <v>1</v>
       </c>
       <c r="L12" s="5">
@@ -5185,27 +5183,27 @@
         <v>4594759.1527198628</v>
       </c>
       <c r="G13" s="71">
-        <f>A13-$A$12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H13" s="21">
-        <f>B13/$B$12</f>
+        <f t="shared" si="1"/>
         <v>0.97862669417140025</v>
       </c>
       <c r="I13" s="5">
-        <f>C13/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.0012022581544466</v>
       </c>
       <c r="J13" s="5">
-        <f>D13/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.0210844828674435</v>
       </c>
       <c r="K13" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.0229231762314899</v>
       </c>
       <c r="L13" s="5">
-        <f t="shared" ref="L13:L32" si="1">F13/$F$12</f>
+        <f t="shared" ref="L13:L32" si="5">F13/$F$12</f>
         <v>1.0232287138610123</v>
       </c>
     </row>
@@ -5232,27 +5230,27 @@
         <v>4592851.1101301583</v>
       </c>
       <c r="G14" s="71">
-        <f>A14-$A$12</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H14" s="21">
-        <f>B14/$B$12</f>
+        <f t="shared" si="1"/>
         <v>0.99070237553418483</v>
       </c>
       <c r="I14" s="5">
-        <f>C14/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.0019236130471145</v>
       </c>
       <c r="J14" s="5">
-        <f>D14/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.0596971479482411</v>
       </c>
       <c r="K14" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.0226100561442151</v>
       </c>
       <c r="L14" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.0228038028047062</v>
       </c>
     </row>
@@ -5279,27 +5277,27 @@
         <v>4984816.060104914</v>
       </c>
       <c r="G15" s="71">
-        <f>A15-$A$12</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H15" s="21">
-        <f>B15/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.0227386912396637</v>
       </c>
       <c r="I15" s="5">
-        <f>C15/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.0084332311123501</v>
       </c>
       <c r="J15" s="5">
-        <f>D15/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.1703636849475125</v>
       </c>
       <c r="K15" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.1102322464387493</v>
       </c>
       <c r="L15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.1100923370478673</v>
       </c>
     </row>
@@ -5326,27 +5324,27 @@
         <v>5059302.2628542436</v>
       </c>
       <c r="G16" s="71">
-        <f>A16-$A$12</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H16" s="21">
-        <f>B16/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.0546035949238399</v>
       </c>
       <c r="I16" s="5">
-        <f>C16/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.0226826038472261</v>
       </c>
       <c r="J16" s="5">
-        <f>D16/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.2756746171943205</v>
       </c>
       <c r="K16" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.1270287190833779</v>
       </c>
       <c r="L16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.1266800229104592</v>
       </c>
     </row>
@@ -5373,27 +5371,27 @@
         <v>5127537.4200238613</v>
       </c>
       <c r="G17" s="71">
-        <f>A17-$A$12</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H17" s="21">
-        <f>B17/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.1000277805689698</v>
       </c>
       <c r="I17" s="5">
-        <f>C17/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.0435775020908837</v>
       </c>
       <c r="J17" s="5">
-        <f>D17/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.2422655511589069</v>
       </c>
       <c r="K17" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.1424144339714173</v>
       </c>
       <c r="L17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.141875633777123</v>
       </c>
     </row>
@@ -5420,27 +5418,27 @@
         <v>5532262.1046198383</v>
       </c>
       <c r="G18" s="71">
-        <f>A18-$A$12</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H18" s="21">
-        <f>B18/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.1291382703935975</v>
       </c>
       <c r="I18" s="5">
-        <f>C18/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.0683196264287707</v>
       </c>
       <c r="J18" s="5">
-        <f>D18/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.2908777646168526</v>
       </c>
       <c r="K18" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.2324433362558471</v>
       </c>
       <c r="L18" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.2320056938569433</v>
       </c>
     </row>
@@ -5467,27 +5465,27 @@
         <v>5275485.7694955673</v>
       </c>
       <c r="G19" s="71">
-        <f>A19-$A$12</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H19" s="21">
-        <f>B19/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.134984011395944</v>
       </c>
       <c r="I19" s="5">
-        <f>C19/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.0959889880122664</v>
       </c>
       <c r="J19" s="5">
-        <f>D19/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.2885477134940848</v>
       </c>
       <c r="K19" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.1758332441525656</v>
       </c>
       <c r="L19" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.1748229536074084</v>
       </c>
     </row>
@@ -5514,27 +5512,27 @@
         <v>5492674.5263839951</v>
       </c>
       <c r="G20" s="71">
-        <f>A20-$A$12</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H20" s="21">
-        <f>B20/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.1617479297565358</v>
       </c>
       <c r="I20" s="5">
-        <f>C20/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.1139392249790911</v>
       </c>
       <c r="J20" s="5">
-        <f>D20/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.3403410595028735</v>
       </c>
       <c r="K20" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.2236660554393917</v>
       </c>
       <c r="L20" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.2231897482509246</v>
       </c>
     </row>
@@ -5561,27 +5559,27 @@
         <v>5639000.7052226886</v>
       </c>
       <c r="G21" s="71">
-        <f>A21-$A$12</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H21" s="21">
-        <f>B21/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.2100092798921878</v>
       </c>
       <c r="I21" s="5">
-        <f>C21/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.1342939782548089</v>
       </c>
       <c r="J21" s="5">
-        <f>D21/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.3387269687270591</v>
       </c>
       <c r="K21" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.2563636877417368</v>
       </c>
       <c r="L21" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.2557758192071538</v>
       </c>
     </row>
@@ -5608,27 +5606,27 @@
         <v>5711477.0863111811</v>
       </c>
       <c r="G22" s="71">
-        <f>A22-$A$12</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="H22" s="21">
-        <f>B22/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.2431095322816121</v>
       </c>
       <c r="I22" s="5">
-        <f>C22/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.1560252299972122</v>
       </c>
       <c r="J22" s="5">
-        <f>D22/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.350606551053589</v>
       </c>
       <c r="K22" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.2722882753220093</v>
       </c>
       <c r="L22" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.2719159283492358</v>
       </c>
     </row>
@@ -5655,27 +5653,27 @@
         <v>5586882.3722885838</v>
       </c>
       <c r="G23" s="71">
-        <f>A23-$A$12</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="H23" s="21">
-        <f>B23/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.2887051299480443</v>
       </c>
       <c r="I23" s="5">
-        <f>C23/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.1797672149428491</v>
       </c>
       <c r="J23" s="5">
-        <f>D23/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.3693591903438846</v>
       </c>
       <c r="K23" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.245219020840683</v>
       </c>
       <c r="L23" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.2441693403898308</v>
       </c>
     </row>
@@ -5702,27 +5700,27 @@
         <v>5997287.4598798994</v>
       </c>
       <c r="G24" s="71">
-        <f>A24-$A$12</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H24" s="21">
-        <f>B24/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.32671131260233</v>
       </c>
       <c r="I24" s="5">
-        <f>C24/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.2125627265124059</v>
       </c>
       <c r="J24" s="5">
-        <f>D24/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.4075982660929032</v>
       </c>
       <c r="K24" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.3360197031591734</v>
       </c>
       <c r="L24" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.335564396361262</v>
       </c>
     </row>
@@ -5749,27 +5747,27 @@
         <v>6361223.2714074589</v>
       </c>
       <c r="G25" s="71">
-        <f>A25-$A$12</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="H25" s="21">
-        <f>B25/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.3871370054910954</v>
       </c>
       <c r="I25" s="5">
-        <f>C25/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.2579174797881238</v>
       </c>
       <c r="J25" s="5">
-        <f>D25/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.501324121509906</v>
       </c>
       <c r="K25" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.4170622080665702</v>
       </c>
       <c r="L25" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.4166109887896972</v>
       </c>
     </row>
@@ -5796,27 +5794,27 @@
         <v>6282762.5923509225</v>
       </c>
       <c r="G26" s="71">
-        <f>A26-$A$12</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="H26" s="21">
-        <f>B26/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.4603358493465655</v>
       </c>
       <c r="I26" s="5">
-        <f>C26/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.314402704209646</v>
       </c>
       <c r="J26" s="5">
-        <f>D26/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.5184945407326125</v>
       </c>
       <c r="K26" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.3995427520911294</v>
       </c>
       <c r="L26" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.3991382079428147</v>
       </c>
     </row>
@@ -5843,27 +5841,27 @@
         <v>6454619.7745619761</v>
       </c>
       <c r="G27" s="71">
-        <f>A27-$A$12</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="H27" s="21">
-        <f>B27/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.5421703126200623</v>
       </c>
       <c r="I27" s="5">
-        <f>C27/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.3844891274045164</v>
       </c>
       <c r="J27" s="5">
-        <f>D27/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.5981624695740144</v>
       </c>
       <c r="K27" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.4384251849680523</v>
       </c>
       <c r="L27" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.4374098991624733</v>
       </c>
     </row>
@@ -5890,27 +5888,27 @@
         <v>6591316.0883027315</v>
       </c>
       <c r="G28" s="71">
-        <f>A28-$A$12</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="H28" s="21">
-        <f>B28/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.6267710112718181</v>
       </c>
       <c r="I28" s="5">
-        <f>C28/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.4726303317535545</v>
       </c>
       <c r="J28" s="5">
-        <f>D28/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.6965749186042138</v>
       </c>
       <c r="K28" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.4686791275267892</v>
       </c>
       <c r="L28" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.4678514497746957</v>
       </c>
     </row>
@@ -5937,27 +5935,27 @@
         <v>6900426.0046540415</v>
       </c>
       <c r="G29" s="71">
-        <f>A29-$A$12</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="H29" s="21">
-        <f>B29/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.6866174497437685</v>
       </c>
       <c r="I29" s="5">
-        <f>C29/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.576303317535545</v>
       </c>
       <c r="J29" s="5">
-        <f>D29/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.7562529512365346</v>
       </c>
       <c r="K29" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.5369459119356834</v>
       </c>
       <c r="L29" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.5366886035050733</v>
       </c>
     </row>
@@ -5984,27 +5982,27 @@
         <v>6789556.1740181493</v>
       </c>
       <c r="G30" s="71">
-        <f>A30-$A$12</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="H30" s="21">
-        <f>B30/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.6613193997032798</v>
       </c>
       <c r="I30" s="5">
-        <f>C30/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.6803038751045443</v>
       </c>
       <c r="J30" s="5">
-        <f>D30/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.7140554190780692</v>
       </c>
       <c r="K30" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.5126247791683525</v>
       </c>
       <c r="L30" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.5119984749397057</v>
       </c>
     </row>
@@ -6031,27 +6029,27 @@
         <v>6791210.1261211922</v>
       </c>
       <c r="G31" s="71">
-        <f>A31-$A$12</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="H31" s="21">
-        <f>B31/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.7094979992079582</v>
       </c>
       <c r="I31" s="5">
-        <f>C31/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.7923264566490102</v>
       </c>
       <c r="J31" s="5">
-        <f>D31/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.655651326002332</v>
       </c>
       <c r="K31" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.5133785482256334</v>
       </c>
       <c r="L31" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.5123668013800988</v>
       </c>
     </row>
@@ -6078,27 +6076,27 @@
         <v>6752336.8930486357</v>
       </c>
       <c r="G32" s="71">
-        <f>A32-$A$12</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="H32" s="21">
-        <f>B32/$B$12</f>
+        <f t="shared" si="1"/>
         <v>1.7624879568278136</v>
       </c>
       <c r="I32" s="5">
-        <f>C32/$C$12</f>
+        <f t="shared" si="2"/>
         <v>1.9066211318650683</v>
       </c>
       <c r="J32" s="65">
-        <f>D32/$D$12</f>
+        <f t="shared" si="3"/>
         <v>1.6753721408566637</v>
       </c>
       <c r="K32" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.5052918416080747</v>
       </c>
       <c r="L32" s="65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.50370993668744</v>
       </c>
     </row>
@@ -11095,22 +11093,17 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="AJ30:AJ31"/>
-    <mergeCell ref="AM30:AM31"/>
-    <mergeCell ref="AN30:AN31"/>
-    <mergeCell ref="AO30:AO31"/>
-    <mergeCell ref="AE30:AE31"/>
-    <mergeCell ref="AF30:AF31"/>
-    <mergeCell ref="AG30:AG31"/>
-    <mergeCell ref="AH30:AH31"/>
-    <mergeCell ref="AI30:AI31"/>
-    <mergeCell ref="AK30:AK31"/>
-    <mergeCell ref="AL30:AL31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="AB30:AB31"/>
+    <mergeCell ref="AC30:AC31"/>
+    <mergeCell ref="AD30:AD31"/>
+    <mergeCell ref="T30:T31"/>
+    <mergeCell ref="U30:U31"/>
+    <mergeCell ref="V30:V31"/>
+    <mergeCell ref="W30:W31"/>
+    <mergeCell ref="X30:X31"/>
+    <mergeCell ref="Y30:Y31"/>
+    <mergeCell ref="Z30:Z31"/>
+    <mergeCell ref="AA30:AA31"/>
     <mergeCell ref="O30:O31"/>
     <mergeCell ref="P30:P31"/>
     <mergeCell ref="S30:S31"/>
@@ -11125,17 +11118,22 @@
     <mergeCell ref="K30:K31"/>
     <mergeCell ref="Q30:Q31"/>
     <mergeCell ref="R30:R31"/>
-    <mergeCell ref="AB30:AB31"/>
-    <mergeCell ref="AC30:AC31"/>
-    <mergeCell ref="AD30:AD31"/>
-    <mergeCell ref="T30:T31"/>
-    <mergeCell ref="U30:U31"/>
-    <mergeCell ref="V30:V31"/>
-    <mergeCell ref="W30:W31"/>
-    <mergeCell ref="X30:X31"/>
-    <mergeCell ref="Y30:Y31"/>
-    <mergeCell ref="Z30:Z31"/>
-    <mergeCell ref="AA30:AA31"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="AJ30:AJ31"/>
+    <mergeCell ref="AM30:AM31"/>
+    <mergeCell ref="AN30:AN31"/>
+    <mergeCell ref="AO30:AO31"/>
+    <mergeCell ref="AE30:AE31"/>
+    <mergeCell ref="AF30:AF31"/>
+    <mergeCell ref="AG30:AG31"/>
+    <mergeCell ref="AH30:AH31"/>
+    <mergeCell ref="AI30:AI31"/>
+    <mergeCell ref="AK30:AK31"/>
+    <mergeCell ref="AL30:AL31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>